<commit_message>
Add Customer Test using Data Driven is Updated
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testData.xlsx
+++ b/src/test/resources/excel/testData.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment_Collection\Eclipse_Env\Workspace\SeleniumDataDrivenFramework\src\test\resources\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99BB1782-2D28-4CB2-B31F-82C05FF89A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="AddCustomer" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,8 +24,31 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>PostCode</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Daniels</t>
+  </si>
+  <si>
+    <t>JD12345</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +359,43 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Dropdown selection functionality added and Common Data provider added
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testData.xlsx
+++ b/src/test/resources/excel/testData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment_Collection\Eclipse_Env\Workspace\SeleniumDataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B78757-F87B-485A-90A0-1F8C92E9D351}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9293FD-02D2-4AE8-8FBC-24B92F2CB942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="AddCustomer" sheetId="1" r:id="rId1"/>
+    <sheet name="addCustomerFlow" sheetId="1" r:id="rId1"/>
+    <sheet name="openAccountFlow" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>FirstName</t>
   </si>
@@ -39,9 +40,6 @@
     <t>Jack</t>
   </si>
   <si>
-    <t>Daniels</t>
-  </si>
-  <si>
     <t>JD12345</t>
   </si>
   <si>
@@ -49,6 +47,24 @@
   </si>
   <si>
     <t>Customer added successfully</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Rupee</t>
+  </si>
+  <si>
+    <t>Account created successfully</t>
+  </si>
+  <si>
+    <t>Harry Potter</t>
   </si>
 </sst>
 </file>
@@ -368,8 +384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,7 +407,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -399,13 +415,54 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{944B8BE9-6F2A-43BA-8CD7-2BE108A0B6CE}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RunMode Config Update and Test Skip Functionality Added
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testData.xlsx
+++ b/src/test/resources/excel/testData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment_Collection\Eclipse_Env\Workspace\SeleniumDataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A251D84-3DFC-4AC2-A9B9-6348DF9528A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1955D4-C47A-4796-9259-20874E636435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="addCustomerFlow" sheetId="1" r:id="rId1"/>
-    <sheet name="openAccountFlow" sheetId="2" r:id="rId2"/>
+    <sheet name="TestSuite" sheetId="3" r:id="rId1"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId2"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>FirstName</t>
   </si>
@@ -89,6 +90,27 @@
   </si>
   <si>
     <t>BE98765</t>
+  </si>
+  <si>
+    <t>TestCaseId</t>
+  </si>
+  <si>
+    <t>RunMode</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>BankManagerLoginTest</t>
+  </si>
+  <si>
+    <t>AddCustomerTest</t>
+  </si>
+  <si>
+    <t>OpenAccountTest</t>
   </si>
 </sst>
 </file>
@@ -104,15 +126,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -120,12 +148,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,11 +450,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{441ED292-DA54-48C6-B808-307C6EE8D48C}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,58 +516,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -481,12 +576,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{944B8BE9-6F2A-43BA-8CD7-2BE108A0B6CE}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,35 +591,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Optimization of Data parameterization using Hashtable is updated
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testData.xlsx
+++ b/src/test/resources/excel/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment_Collection\Eclipse_Env\Workspace\SeleniumDataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1955D4-C47A-4796-9259-20874E636435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20582804-8F64-4021-9BF5-7F87766853C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>FirstName</t>
   </si>
@@ -167,10 +167,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,7 +454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{441ED292-DA54-48C6-B808-307C6EE8D48C}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -501,10 +502,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,7 +516,7 @@
     <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -528,8 +529,11 @@
       <c r="D1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -542,8 +546,11 @@
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -556,8 +563,11 @@
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -569,6 +579,9 @@
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Extent Report Screenshot Update Issue Fix
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testData.xlsx
+++ b/src/test/resources/excel/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment_Collection\Eclipse_Env\Workspace\SeleniumDataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20582804-8F64-4021-9BF5-7F87766853C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654F75A0-9671-4536-8F78-D09A297A9EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>FirstName</t>
   </si>
@@ -99,9 +99,6 @@
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>BankManagerLoginTest</t>
@@ -167,11 +164,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,7 +450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{441ED292-DA54-48C6-B808-307C6EE8D48C}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -473,7 +469,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>23</v>
@@ -481,7 +477,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>23</v>
@@ -489,10 +485,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -504,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,7 +542,7 @@
       <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>23</v>
       </c>
     </row>
@@ -563,8 +559,8 @@
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>24</v>
+      <c r="E3" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -580,7 +576,7 @@
       <c r="D4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="1" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Selenium Grid TestData Update
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testData.xlsx
+++ b/src/test/resources/excel/testData.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment_Collection\Eclipse_Env\Workspace\SeleniumDataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654F75A0-9671-4536-8F78-D09A297A9EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A49E88-C368-4D09-B8A1-AA84AFA31E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="3" r:id="rId1"/>
-    <sheet name="AddCustomerTest" sheetId="1" r:id="rId2"/>
-    <sheet name="OpenAccountTest" sheetId="2" r:id="rId3"/>
+    <sheet name="TestSuiteGrid" sheetId="4" r:id="rId2"/>
+    <sheet name="AddCustomerTest" sheetId="1" r:id="rId3"/>
+    <sheet name="AddCustomerTestGrid" sheetId="5" r:id="rId4"/>
+    <sheet name="OpenAccountTest" sheetId="2" r:id="rId5"/>
+    <sheet name="OpenAccountTestGrid" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="27">
   <si>
     <t>FirstName</t>
   </si>
@@ -497,6 +500,56 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38BF4B6F-BD57-4462-8CD0-37877B32A8D7}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
@@ -585,7 +638,96 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB72C106-3EF3-450E-85D8-5BC5783E7C7F}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{944B8BE9-6F2A-43BA-8CD7-2BE108A0B6CE}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -636,4 +778,57 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C278846-916C-40F0-B41C-050D3B7D9BF2}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Selenium Grid Integatio Code Sequential Execution Working
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testData.xlsx
+++ b/src/test/resources/excel/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Environment_Collection\Eclipse_Env\Workspace\SeleniumDataDrivenFramework\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07A49E88-C368-4D09-B8A1-AA84AFA31E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56629DC-CEE3-4DDD-8890-6D16ADED71FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="3" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="30">
   <si>
     <t>FirstName</t>
   </si>
@@ -111,6 +111,15 @@
   </si>
   <si>
     <t>OpenAccountTest</t>
+  </si>
+  <si>
+    <t>BankManagerLoginTestGrid</t>
+  </si>
+  <si>
+    <t>AddCustomerTestGrid</t>
+  </si>
+  <si>
+    <t>OpenAccountTestGrid</t>
   </si>
 </sst>
 </file>
@@ -453,6 +462,56 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{441ED292-DA54-48C6-B808-307C6EE8D48C}">
   <dimension ref="A1:B4"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38BF4B6F-BD57-4462-8CD0-37877B32A8D7}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
@@ -472,7 +531,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>23</v>
@@ -480,7 +539,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>23</v>
@@ -488,57 +547,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38BF4B6F-BD57-4462-8CD0-37877B32A8D7}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>23</v>

</xml_diff>